<commit_message>
CCSB Loads, Outflow, wy2016-18, pTHg, fTHg, wwTHg: Updated the Outflow Q and WQ worksheet; Updated the model results sheets; replaced rloadest folders; replaced the Sigma Plot file and PDFs; added Powerpoint files to the Sigma Plot folder.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/4_wy2016-2018/4_fTHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/4_wy2016-2018/4_fTHg Model Results.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\4_wy2016-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A35E4E-ABA7-4DCF-AD79-83EC1B3A1505}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731B8989-49D2-42CB-8921-7A1619471FFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28995" yWindow="12915" windowWidth="15285" windowHeight="11385" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fTHg wy2016-18 Model Results" sheetId="2" r:id="rId1"/>
-    <sheet name="Outlet" sheetId="5" r:id="rId2"/>
+    <sheet name="Outlet_30ct" sheetId="5" r:id="rId2"/>
     <sheet name="Rumsey" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="469">
   <si>
     <t>Model #</t>
   </si>
@@ -906,60 +906,12 @@
     <t>Station: CCSB-Yolo</t>
   </si>
   <si>
-    <t xml:space="preserve">           Number of Observations: 31</t>
-  </si>
-  <si>
-    <t>Number of Uncensored Observations: 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           Center of Decimal Time: 2016.949</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  Center of ln(Q): 5.555</t>
-  </si>
-  <si>
     <t xml:space="preserve">                 Period of record: 2016-01-20 to 2018-04-08</t>
   </si>
   <si>
-    <t>(Intercept)   -5.762    0.13576  -42.44       0</t>
-  </si>
-  <si>
-    <t>lnQ            1.013    0.05731   17.67       0</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.4413</t>
-  </si>
-  <si>
-    <t>R-squared: 91.5 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 76.42 on 1 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.018</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.5146</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.18 0.21 0.22</t>
-  </si>
-  <si>
     <t>Obs   0   0 0.01 0.06 0.17 0.28 0.31</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bp: -6.67 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.9333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.8809</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm2 &lt;- loadReg(fTHg ~model(2), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -969,45 +921,6 @@
     <t>&gt; fTHg_Outflowm2</t>
   </si>
   <si>
-    <t>(Intercept) -5.92697    0.15328 -38.669  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ          1.01266    0.05455  18.562  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2         0.02939    0.01469   2.001  0.0418</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.3999</t>
-  </si>
-  <si>
-    <t>R-squared: 92.56 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 80.57 on 2 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9696</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0787</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.6216</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.23 0.28 0.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 9.975 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.887</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm3 &lt;- loadReg(fTHg ~model(3), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1017,54 +930,6 @@
     <t>&gt; fTHg_Outflowm3</t>
   </si>
   <si>
-    <t>(Intercept)  -5.9172    0.12255 -48.284   0e+00</t>
-  </si>
-  <si>
-    <t>lnQ           1.0117    0.04837  20.919   0e+00</t>
-  </si>
-  <si>
-    <t>DECTIME      -0.5838    0.16370  -3.566   7e-04</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.3143</t>
-  </si>
-  <si>
-    <t>R-squared: 94.16 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 88.03 on 2 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9881</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.6102</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.2913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        VIF</t>
-  </si>
-  <si>
-    <t>lnQ       1</t>
-  </si>
-  <si>
-    <t>DECTIME   1</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.13 0.15 0.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: -20.03 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.7997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.7716</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm4 &lt;- loadReg(fTHg ~model(4), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1074,57 +939,6 @@
     <t>&gt; fTHg_Outflowm4</t>
   </si>
   <si>
-    <t>(Intercept)  -6.5887    0.58564 -11.2503  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           0.9926    0.06092  16.2948  0.0000</t>
-  </si>
-  <si>
-    <t>sin.DECTIME   0.3843    0.54669   0.7029  0.4534</t>
-  </si>
-  <si>
-    <t>cos.DECTIME   1.1060    0.52815   2.0941  0.0308</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.359</t>
-  </si>
-  <si>
-    <t>R-squared: 93.56 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 85.03 on 3 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0546</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.3204</t>
-  </si>
-  <si>
-    <t>lnQ         1.389</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 4.070</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 3.646</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.21 0.23 0.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 0.9865 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.9151</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm5 &lt;- loadReg(fTHg ~model(5), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1134,57 +948,6 @@
     <t>&gt; fTHg_Outflowm5</t>
   </si>
   <si>
-    <t>(Intercept)  -6.1744    0.12331 -50.074   0e+00</t>
-  </si>
-  <si>
-    <t>lnQ           1.0116    0.04015  25.195   0e+00</t>
-  </si>
-  <si>
-    <t>lnQ2          0.0408    0.01105   3.692   4e-04</t>
-  </si>
-  <si>
-    <t>DECTIME      -0.6904    0.13892  -4.970   0e+00</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.2166</t>
-  </si>
-  <si>
-    <t>R-squared: 96.12 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 100.7 on 3 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.096</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.2503</t>
-  </si>
-  <si>
-    <t>lnQ     1.000</t>
-  </si>
-  <si>
-    <t>lnQ2    1.045</t>
-  </si>
-  <si>
-    <t>DECTIME 1.045</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.17 0.21 0.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: -4.961 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.9504</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.9054</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm6 &lt;- loadReg(fTHg ~model(6), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1194,63 +957,6 @@
     <t>&gt; fTHg_Outflowm6</t>
   </si>
   <si>
-    <t>(Intercept) -6.77018    0.59114 -11.4528  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ          0.98369    0.06029  16.3161  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2         0.02046    0.01488   1.3751  0.1402</t>
-  </si>
-  <si>
-    <t>sin.DECTIME  0.52817    0.54798   0.9639  0.2968</t>
-  </si>
-  <si>
-    <t>cos.DECTIME  1.08308    0.51992   2.0832  0.0287</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.3476</t>
-  </si>
-  <si>
-    <t>R-squared: 94 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 87.21 on 4 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9647</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0456</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.4002</t>
-  </si>
-  <si>
-    <t>lnQ         1.405</t>
-  </si>
-  <si>
-    <t>lnQ2        1.181</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 4.224</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 3.649</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.24 0.27 0.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 10.65 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.8743</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm7 &lt;- loadReg(fTHg ~model(7), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1260,63 +966,6 @@
     <t>&gt; fTHg_Outflowm7</t>
   </si>
   <si>
-    <t>(Intercept)  -5.8509    0.55414 -10.5586  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           1.0368    0.05424  19.1133  0.0000</t>
-  </si>
-  <si>
-    <t>DECTIME      -0.5580    0.17324  -3.2208  0.0013</t>
-  </si>
-  <si>
-    <t>sin.DECTIME  -0.3900    0.52880  -0.7374  0.4231</t>
-  </si>
-  <si>
-    <t>cos.DECTIME   0.2803    0.52228   0.5368  0.5589</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.2665</t>
-  </si>
-  <si>
-    <t>R-squared: 95.4 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 95.44 on 4 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9812</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.2918</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.2015</t>
-  </si>
-  <si>
-    <t>lnQ         1.483</t>
-  </si>
-  <si>
-    <t>DECTIME     1.321</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 5.130</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 4.803</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.15 0.21 0.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: -12.89 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.8711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.9156</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm8 &lt;- loadReg(fTHg ~model(8), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1326,69 +975,9 @@
     <t>&gt; fTHg_Outflowm8</t>
   </si>
   <si>
-    <t>(Intercept) -5.99776    0.49754 -12.0548  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ          1.03107    0.04847  21.2730  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2         0.03319    0.01202   2.7611  0.0041</t>
-  </si>
-  <si>
-    <t>DECTIME     -0.66960    0.15985  -4.1888  0.0000</t>
-  </si>
-  <si>
-    <t>sin.DECTIME -0.31133    0.47294  -0.6583  0.4655</t>
-  </si>
-  <si>
-    <t>cos.DECTIME  0.07797    0.47198   0.1652  0.8541</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.2124</t>
-  </si>
-  <si>
-    <t>R-squared: 96.47 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 103.7 on 5 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.1207</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.2841</t>
-  </si>
-  <si>
-    <t>lnQ         1.486</t>
-  </si>
-  <si>
     <t>lnQ2        1.261</t>
   </si>
   <si>
-    <t>DECTIME     1.411</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 5.149</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 4.922</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.17 0.23 0.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: -2.894 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.9711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.9556</t>
-  </si>
-  <si>
     <t>&gt; fTHg_Outflowm9 &lt;- loadReg(fTHg ~model(9), data = fTHg_Outflow, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -1398,88 +987,496 @@
     <t>&gt; fTHg_Outflowm9</t>
   </si>
   <si>
-    <t>(Intercept) -5.72821    0.48621 -11.781  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ          1.10306    0.05749  19.186  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2         0.04575    0.01286   3.559  0.0003</t>
-  </si>
-  <si>
-    <t>DECTIME     -0.78971    0.16137  -4.894  0.0000</t>
-  </si>
-  <si>
-    <t>DECTIME2     0.55842    0.27150   2.057  0.0249</t>
-  </si>
-  <si>
-    <t>sin.DECTIME -1.00984    0.55983  -1.804  0.0471</t>
-  </si>
-  <si>
-    <t>cos.DECTIME -0.41234    0.50409  -0.818  0.3559</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.1881</t>
-  </si>
-  <si>
-    <t>R-squared: 97 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 108.7 on 6 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9783</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.2111</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.3331</t>
-  </si>
-  <si>
-    <t>lnQ2        1.629</t>
-  </si>
-  <si>
-    <t>DECTIME     1.624</t>
-  </si>
-  <si>
-    <t>DECTIME2    2.364</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 8.147</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 6.339</t>
-  </si>
-  <si>
-    <t>Est   0   0 0.01 0.06 0.15 0.27 0.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: -1.05 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.9895</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.9723</t>
-  </si>
-  <si>
-    <t>Number of Uncensored Observations: 31; Period of record: 2016-01-20 to 2018-04-08</t>
-  </si>
-  <si>
-    <t>15.76, 14.43, 13.50</t>
-  </si>
-  <si>
-    <t>15.86, 16.11, 18.96</t>
-  </si>
-  <si>
-    <t>12.45, 15.32, 28.17</t>
-  </si>
-  <si>
-    <t>12.49, 15.53, 28.63</t>
-  </si>
-  <si>
-    <t>n-close</t>
+    <t xml:space="preserve">           Number of Observations: 30</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 6.989</t>
+  </si>
+  <si>
+    <t>(Intercept)   -4.337    0.11510  -37.68       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.104    0.07006   15.75       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3968</t>
+  </si>
+  <si>
+    <t>R-squared: 89.86 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 68.67 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0278</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5438</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.22 0.25 0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 5.494 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.899</t>
+  </si>
+  <si>
+    <t>(Intercept) -4.357980    0.17318 -25.1641  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.103780    0.07131  15.4781  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.007756    0.04726   0.1641  0.8627</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.4111</t>
+  </si>
+  <si>
+    <t>R-squared: 89.87 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 68.7 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0358</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5648</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.22 0.26 0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 6.699 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8974</t>
+  </si>
+  <si>
+    <t>(Intercept)  -4.5138    0.09848 -45.835   0e+00</t>
+  </si>
+  <si>
+    <t>lnQ           1.1183    0.05474  20.429   0e+00</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.6292    0.14422  -4.363   1e-04</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.2414</t>
+  </si>
+  <si>
+    <t>R-squared: 94.05 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 84.68 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0483</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.1793</t>
+  </si>
+  <si>
+    <t>lnQ     1.004</t>
+  </si>
+  <si>
+    <t>DECTIME 1.004</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.07 0.17 0.18 0.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -10.2 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8571</t>
+  </si>
+  <si>
+    <t>(Intercept)  -5.2465    0.60811 -8.6277  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.0569    0.07019 15.0572  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.4953    0.53304  0.9293  0.3222</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   1.0860    0.51116  2.1247  0.0284</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3361</t>
+  </si>
+  <si>
+    <t>R-squared: 92.03 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 75.87 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0306</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3448</t>
+  </si>
+  <si>
+    <t>lnQ         1.185</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.475</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.508</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.24 0.26 0.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 9.107 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8862</t>
+  </si>
+  <si>
+    <t>(Intercept) -4.73811    0.14733 -32.159  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.12063    0.05204  21.533  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.07252    0.03678   1.972  0.0409</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.73113    0.14649  -4.991  0.0000</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.218</t>
+  </si>
+  <si>
+    <t>R-squared: 94.83 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 88.86 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.3844</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3285</t>
+  </si>
+  <si>
+    <t>lnQ2    1.142</t>
+  </si>
+  <si>
+    <t>DECTIME 1.146</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.20 0.22 0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -1.872 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.9216</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.10657    0.64903 -7.8680  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.05854    0.07099 14.9116  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.03256    0.04849 -0.6714  0.4640</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.40597    0.55496  0.7315  0.4254</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  1.09742    0.51692  2.1230  0.0258</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3434</t>
+  </si>
+  <si>
+    <t>R-squared: 92.17 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 76.41 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0144</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2446</t>
+  </si>
+  <si>
+    <t>lnQ         1.186</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.687</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.512</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.22 0.24 0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 3.873 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.9114</t>
+  </si>
+  <si>
+    <t>(Intercept)  -4.3983    0.54113 -8.1280  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.1189    0.05921 18.8963  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.6056    0.15893 -3.8107  0.0002</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -0.3206    0.48246 -0.6644  0.4687</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   0.1854    0.47723  0.3886  0.6708</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.2211</t>
+  </si>
+  <si>
+    <t>R-squared: 94.96 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 89.61 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0229</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.1661</t>
+  </si>
+  <si>
+    <t>lnQ         1.282</t>
+  </si>
+  <si>
+    <t>DECTIME     1.331</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.327</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 4.648</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.17 0.22 0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -6.059 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.943</t>
+  </si>
+  <si>
+    <t>(Intercept) -4.47384    0.54524 -8.20520  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.12535    0.05945 18.92845  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.04534    0.04377  1.03572  0.2521</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.69091    0.17879 -3.86445  0.0001</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.31099    0.48185 -0.64540  0.4725</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.04280    0.49604  0.08629  0.9232</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.2205</t>
+  </si>
+  <si>
+    <t>R-squared: 95.17 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 90.92 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.28</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2995</t>
+  </si>
+  <si>
+    <t>lnQ         1.296</t>
+  </si>
+  <si>
+    <t>lnQ2        1.600</t>
+  </si>
+  <si>
+    <t>DECTIME     1.689</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.329</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.036</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.19 0.24 0.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -1.808 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.9577</t>
+  </si>
+  <si>
+    <t>(Intercept) -4.07147    0.55187 -7.3776  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.23311    0.07770 15.8696  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.05376    0.04148  1.2960  0.1459</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.79707    0.17668 -4.5114  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME2     0.55552    0.27746  2.0022  0.0281</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.00599    0.57167 -1.7597  0.0516</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.43316    0.52455 -0.8258  0.3492</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1959</t>
+  </si>
+  <si>
+    <t>R-squared: 95.89 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 95.74 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.3248</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3437</t>
+  </si>
+  <si>
+    <t>lnQ         2.491</t>
+  </si>
+  <si>
+    <t>lnQ2        1.616</t>
+  </si>
+  <si>
+    <t>DECTIME     1.856</t>
+  </si>
+  <si>
+    <t>DECTIME2    2.288</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.857</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 6.337</t>
+  </si>
+  <si>
+    <t>Est   0   0 0.01 0.06 0.17 0.27 0.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -0.2622 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.9727</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 30; Period of record: 2016-01-20 to 2018-04-08</t>
+  </si>
+  <si>
+    <t>13.1, 17.7, 20.5</t>
+  </si>
+  <si>
+    <t>12.1, 14.8, 29.2</t>
+  </si>
+  <si>
+    <t>11.6, 14.3, 45.5</t>
+  </si>
+  <si>
+    <t>2 of 3</t>
+  </si>
+  <si>
+    <t>1 of 3</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1846,6 +1843,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1870,7 +1870,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2344,7 +2353,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O18" sqref="O17:O18"/>
+      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,24 +2375,24 @@
       <c r="A1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46" t="s">
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="46"/>
+      <c r="M1" s="47"/>
       <c r="O1" s="21"/>
       <c r="R1" s="8" t="s">
         <v>10</v>
@@ -2434,7 +2443,7 @@
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
       <c r="R2" s="8" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -2524,39 +2533,39 @@
       <c r="Q5" s="37"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>272</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="54"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
-        <v>464</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="47" t="s">
+      <c r="B7" s="49" t="s">
+        <v>463</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="47"/>
+      <c r="M7" s="48"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:31" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -2641,19 +2650,19 @@
         <v>7</v>
       </c>
       <c r="I9" s="6">
-        <v>91.5</v>
+        <v>89.86</v>
       </c>
       <c r="J9" s="6">
-        <v>1.7999999999999999E-2</v>
+        <v>2.7799999999999998E-2</v>
       </c>
       <c r="K9" s="6">
-        <v>0.51459999999999995</v>
+        <v>0.54379999999999995</v>
       </c>
       <c r="L9" s="6">
-        <v>-6.67</v>
+        <v>5.4939999999999998</v>
       </c>
       <c r="M9" s="6">
-        <v>0.88090000000000002</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="N9" s="6">
         <v>1</v>
@@ -2662,9 +2671,11 @@
         <v>267</v>
       </c>
       <c r="P9" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="Q9" s="31"/>
+        <v>464</v>
+      </c>
+      <c r="Q9" s="31" t="s">
+        <v>468</v>
+      </c>
       <c r="R9" s="8" t="s">
         <v>10</v>
       </c>
@@ -2684,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="19">
-        <v>4.1799999999999997E-2</v>
+        <v>0.86270000000000002</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>9</v>
@@ -2701,36 +2712,32 @@
       <c r="H10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="45">
-        <v>92.56</v>
-      </c>
-      <c r="J10" s="45">
-        <v>7.8700000000000006E-2</v>
-      </c>
-      <c r="K10" s="45">
-        <v>0.62160000000000004</v>
-      </c>
-      <c r="L10" s="45">
-        <v>9.9749999999999996</v>
-      </c>
-      <c r="M10" s="45">
-        <v>0.88700000000000001</v>
+      <c r="I10" s="46">
+        <v>89.87</v>
+      </c>
+      <c r="J10" s="46">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="K10" s="46">
+        <v>0.56479999999999997</v>
+      </c>
+      <c r="L10" s="46">
+        <v>6.6989999999999998</v>
+      </c>
+      <c r="M10" s="46">
+        <v>0.89739999999999998</v>
       </c>
       <c r="N10" s="6">
         <v>2</v>
       </c>
-      <c r="O10" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="P10" s="40" t="s">
-        <v>466</v>
-      </c>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
       <c r="Q10" s="31"/>
       <c r="R10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>11</v>
@@ -2738,60 +2745,62 @@
       <c r="AE10" s="9"/>
     </row>
     <row r="11" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="31">
+      <c r="A11" s="56">
         <v>3</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="56">
         <v>0</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="32">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="57">
+        <v>1E-4</v>
+      </c>
+      <c r="E11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="31">
-        <v>94.16</v>
-      </c>
-      <c r="J11" s="31">
-        <v>0.61019999999999996</v>
-      </c>
-      <c r="K11" s="31">
-        <v>0.2913</v>
-      </c>
-      <c r="L11" s="31">
-        <v>-20.03</v>
-      </c>
-      <c r="M11" s="31">
-        <v>0.77159999999999995</v>
-      </c>
-      <c r="N11" s="31">
+      <c r="I11" s="56">
+        <v>94.05</v>
+      </c>
+      <c r="J11" s="56">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="K11" s="56">
+        <v>0.17929999999999999</v>
+      </c>
+      <c r="L11" s="56">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="M11" s="56">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="N11" s="44">
         <v>3</v>
       </c>
-      <c r="O11" s="31" t="s">
+      <c r="O11" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="P11" s="31" t="s">
+      <c r="P11" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q11" s="58" t="s">
         <v>467</v>
       </c>
-      <c r="Q11" s="31"/>
       <c r="R11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="AB11" s="9" t="s">
         <v>11</v>
@@ -2815,28 +2824,28 @@
         <v>9</v>
       </c>
       <c r="F12" s="6">
-        <v>0.45340000000000003</v>
-      </c>
-      <c r="G12" s="45">
-        <v>3.0800000000000001E-2</v>
+        <v>0.32219999999999999</v>
+      </c>
+      <c r="G12" s="46">
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="45">
-        <v>93.56</v>
-      </c>
-      <c r="J12" s="45">
-        <v>5.4600000000000003E-2</v>
-      </c>
-      <c r="K12" s="45">
-        <v>0.32040000000000002</v>
-      </c>
-      <c r="L12" s="45">
-        <v>0.98650000000000004</v>
-      </c>
-      <c r="M12" s="45">
-        <v>0.91510000000000002</v>
+      <c r="I12" s="46">
+        <v>92.03</v>
+      </c>
+      <c r="J12" s="46">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="K12" s="46">
+        <v>0.3448</v>
+      </c>
+      <c r="L12" s="46">
+        <v>9.1069999999999993</v>
+      </c>
+      <c r="M12" s="46">
+        <v>0.88619999999999999</v>
       </c>
       <c r="N12" s="31">
         <v>4</v>
@@ -2847,7 +2856,7 @@
         <v>10</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>332</v>
+        <v>287</v>
       </c>
       <c r="AB12" s="9" t="s">
         <v>11</v>
@@ -2855,62 +2864,62 @@
       <c r="AE12" s="9"/>
     </row>
     <row r="13" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
+      <c r="A13" s="6">
         <v>5</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="6">
         <v>0</v>
       </c>
-      <c r="C13" s="54">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="D13" s="54">
+      <c r="C13" s="55">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="D13" s="55">
         <v>0</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="11">
-        <v>96.12</v>
-      </c>
-      <c r="J13" s="11">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="K13" s="11">
-        <v>0.25030000000000002</v>
-      </c>
-      <c r="L13" s="11">
-        <v>-4.9610000000000003</v>
-      </c>
-      <c r="M13" s="45">
-        <v>0.90539999999999998</v>
-      </c>
-      <c r="N13" s="44">
+      <c r="I13" s="6">
+        <v>94.83</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.32850000000000001</v>
+      </c>
+      <c r="L13" s="6">
+        <v>-1.8720000000000001</v>
+      </c>
+      <c r="M13" s="46">
+        <v>0.92159999999999997</v>
+      </c>
+      <c r="N13" s="31">
         <v>5</v>
       </c>
-      <c r="O13" s="44" t="s">
+      <c r="O13" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="P13" s="44" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q13" s="44" t="s">
-        <v>469</v>
+      <c r="P13" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>271</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="AB13" s="9" t="s">
         <v>11</v>
@@ -2924,8 +2933,8 @@
       <c r="B14" s="6">
         <v>0</v>
       </c>
-      <c r="C14" s="45">
-        <v>0.14019999999999999</v>
+      <c r="C14" s="46">
+        <v>0.46400000000000002</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>9</v>
@@ -2934,28 +2943,28 @@
         <v>9</v>
       </c>
       <c r="F14" s="6">
-        <v>0.29680000000000001</v>
-      </c>
-      <c r="G14" s="45">
-        <v>2.87E-2</v>
+        <v>0.4254</v>
+      </c>
+      <c r="G14" s="46">
+        <v>2.58E-2</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="45">
-        <v>94</v>
-      </c>
-      <c r="J14" s="45">
-        <v>4.5600000000000002E-2</v>
-      </c>
-      <c r="K14" s="45">
-        <v>0.4002</v>
-      </c>
-      <c r="L14" s="45">
-        <v>10.65</v>
-      </c>
-      <c r="M14" s="45">
-        <v>0.87429999999999997</v>
+      <c r="I14" s="46">
+        <v>92.17</v>
+      </c>
+      <c r="J14" s="46">
+        <v>1.44E-2</v>
+      </c>
+      <c r="K14" s="46">
+        <v>0.24460000000000001</v>
+      </c>
+      <c r="L14" s="46">
+        <v>3.8730000000000002</v>
+      </c>
+      <c r="M14" s="46">
+        <v>0.91139999999999999</v>
       </c>
       <c r="N14" s="31">
         <v>6</v>
@@ -2966,7 +2975,7 @@
         <v>10</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>372</v>
+        <v>293</v>
       </c>
       <c r="AB14" s="9" t="s">
         <v>11</v>
@@ -2984,34 +2993,34 @@
         <v>9</v>
       </c>
       <c r="D15" s="6">
-        <v>1.2999999999999999E-3</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="6">
-        <v>0.42309999999999998</v>
-      </c>
-      <c r="G15" s="45">
-        <v>0.55889999999999995</v>
+        <v>0.46870000000000001</v>
+      </c>
+      <c r="G15" s="46">
+        <v>0.67079999999999995</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="45">
-        <v>95.4</v>
-      </c>
-      <c r="J15" s="45">
-        <v>0.2918</v>
-      </c>
-      <c r="K15" s="45">
-        <v>0.20150000000000001</v>
-      </c>
-      <c r="L15" s="45">
-        <v>-12.89</v>
-      </c>
-      <c r="M15" s="45">
-        <v>0.91559999999999997</v>
+      <c r="I15" s="46">
+        <v>94.96</v>
+      </c>
+      <c r="J15" s="46">
+        <v>2.29E-2</v>
+      </c>
+      <c r="K15" s="46">
+        <v>0.1661</v>
+      </c>
+      <c r="L15" s="46">
+        <v>-6.0590000000000002</v>
+      </c>
+      <c r="M15" s="46">
+        <v>0.94299999999999995</v>
       </c>
       <c r="N15" s="31">
         <v>7</v>
@@ -3022,7 +3031,7 @@
         <v>10</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>394</v>
+        <v>296</v>
       </c>
       <c r="AB15" s="9" t="s">
         <v>11</v>
@@ -3036,38 +3045,38 @@
       <c r="B16" s="6">
         <v>0</v>
       </c>
-      <c r="C16" s="45">
-        <v>4.1000000000000003E-3</v>
+      <c r="C16" s="46">
+        <v>0.25209999999999999</v>
       </c>
       <c r="D16" s="6">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="6">
-        <v>0.46550000000000002</v>
+        <v>0.47249999999999998</v>
       </c>
       <c r="G16" s="6">
-        <v>0.85409999999999997</v>
+        <v>0.92320000000000002</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="45">
-        <v>96.47</v>
-      </c>
-      <c r="J16" s="45">
-        <v>0.1207</v>
-      </c>
-      <c r="K16" s="45">
-        <v>0.28410000000000002</v>
-      </c>
-      <c r="L16" s="45">
-        <v>-2.8940000000000001</v>
-      </c>
-      <c r="M16" s="45">
-        <v>0.9556</v>
+      <c r="I16" s="46">
+        <v>95.17</v>
+      </c>
+      <c r="J16" s="46">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K16" s="46">
+        <v>0.29949999999999999</v>
+      </c>
+      <c r="L16" s="46">
+        <v>-1.8080000000000001</v>
+      </c>
+      <c r="M16" s="46">
+        <v>0.9577</v>
       </c>
       <c r="N16" s="31">
         <v>8</v>
@@ -3078,7 +3087,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>416</v>
+        <v>299</v>
       </c>
       <c r="AB16" s="9" t="s">
         <v>11</v>
@@ -3092,38 +3101,38 @@
       <c r="B17" s="6">
         <v>0</v>
       </c>
-      <c r="C17" s="45">
-        <v>2.9999999999999997E-4</v>
+      <c r="C17" s="46">
+        <v>0.1459</v>
       </c>
       <c r="D17" s="6">
         <v>0</v>
       </c>
       <c r="E17" s="6">
-        <v>2.4899999999999999E-2</v>
+        <v>2.81E-2</v>
       </c>
       <c r="F17" s="6">
-        <v>4.7100000000000003E-2</v>
+        <v>5.16E-2</v>
       </c>
       <c r="G17" s="6">
-        <v>0.35589999999999999</v>
+        <v>0.34920000000000001</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="45">
-        <v>97</v>
-      </c>
-      <c r="J17" s="45">
-        <v>0.21110000000000001</v>
-      </c>
-      <c r="K17" s="45">
-        <v>0.33310000000000001</v>
-      </c>
-      <c r="L17" s="45">
-        <v>-1.05</v>
-      </c>
-      <c r="M17" s="45">
-        <v>0.97230000000000005</v>
+      <c r="I17" s="46">
+        <v>95.89</v>
+      </c>
+      <c r="J17" s="46">
+        <v>0.32479999999999998</v>
+      </c>
+      <c r="K17" s="46">
+        <v>0.34370000000000001</v>
+      </c>
+      <c r="L17" s="46">
+        <v>-0.26219999999999999</v>
+      </c>
+      <c r="M17" s="46">
+        <v>0.97270000000000001</v>
       </c>
       <c r="N17" s="31">
         <v>9</v>
@@ -3134,7 +3143,7 @@
         <v>10</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>440</v>
+        <v>303</v>
       </c>
       <c r="AB17" s="9" t="s">
         <v>11</v>
@@ -3142,39 +3151,39 @@
       <c r="AE17" s="9"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="47" t="s">
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="47"/>
+      <c r="M20" s="48"/>
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:31" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -3817,7 +3826,7 @@
   <dimension ref="A1:A528"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3870,27 +3879,27 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -3929,12 +3938,12 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -3947,17 +3956,17 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -3972,17 +3981,17 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -4018,12 +4027,12 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
@@ -4041,17 +4050,17 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
@@ -4059,7 +4068,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -4069,7 +4078,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
@@ -4079,7 +4088,7 @@
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -4105,27 +4114,27 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
@@ -4159,22 +4168,22 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>69</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>299</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
@@ -4187,17 +4196,17 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
@@ -4212,17 +4221,17 @@
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>306</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
@@ -4278,12 +4287,12 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
@@ -4301,17 +4310,17 @@
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4319,7 +4328,7 @@
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
@@ -4329,7 +4338,7 @@
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
@@ -4339,7 +4348,7 @@
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
@@ -4365,27 +4374,27 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
@@ -4424,17 +4433,17 @@
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
@@ -4447,17 +4456,17 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
@@ -4472,17 +4481,17 @@
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>322</v>
+        <v>341</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -4495,17 +4504,17 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>324</v>
+        <v>124</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
@@ -4538,12 +4547,12 @@
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
@@ -4561,17 +4570,17 @@
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>329</v>
+        <v>347</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
@@ -4579,7 +4588,7 @@
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="15" t="s">
-        <v>331</v>
+        <v>286</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
@@ -4589,7 +4598,7 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>332</v>
+        <v>287</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
@@ -4599,7 +4608,7 @@
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="15" t="s">
-        <v>333</v>
+        <v>288</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
@@ -4625,27 +4634,27 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
@@ -4679,27 +4688,27 @@
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
@@ -4712,17 +4721,17 @@
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="14" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="14" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
@@ -4737,17 +4746,17 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="14" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="14" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
@@ -4765,17 +4774,17 @@
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="14" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="14" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="14" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
@@ -4808,12 +4817,12 @@
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="14" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
@@ -4831,17 +4840,17 @@
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="14" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="14" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="14" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
@@ -4849,7 +4858,7 @@
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="15" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
@@ -4859,7 +4868,7 @@
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
@@ -4869,7 +4878,7 @@
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="15" t="s">
-        <v>353</v>
+        <v>291</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
@@ -4895,27 +4904,27 @@
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
@@ -4954,22 +4963,22 @@
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="14" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="14" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="14" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="14" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
@@ -4982,17 +4991,17 @@
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="14" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="14" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="14" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
@@ -5007,17 +5016,17 @@
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="14" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="14" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="14" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
@@ -5035,17 +5044,17 @@
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="14" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="14" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="14" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
@@ -5078,12 +5087,12 @@
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="14" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
@@ -5101,17 +5110,17 @@
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="14" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="14" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="14" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
@@ -5119,7 +5128,7 @@
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="15" t="s">
-        <v>371</v>
+        <v>292</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
@@ -5129,7 +5138,7 @@
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
-        <v>372</v>
+        <v>293</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
@@ -5139,7 +5148,7 @@
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="15" t="s">
-        <v>373</v>
+        <v>294</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
@@ -5165,27 +5174,27 @@
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
@@ -5219,32 +5228,32 @@
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="14" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="14" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="14" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="14" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="14" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="14" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
@@ -5257,17 +5266,17 @@
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="14" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="14" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="14" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
@@ -5282,17 +5291,17 @@
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="14" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="14" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="14" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
@@ -5310,22 +5319,22 @@
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="14" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="14" t="s">
-        <v>386</v>
+        <v>301</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="14" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="14" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
@@ -5358,12 +5367,12 @@
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="14" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
@@ -5381,17 +5390,17 @@
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="14" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="14" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="14" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
@@ -5399,7 +5408,7 @@
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="15" t="s">
-        <v>393</v>
+        <v>295</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
@@ -5409,7 +5418,7 @@
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="7" t="s">
-        <v>394</v>
+        <v>296</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
@@ -5419,7 +5428,7 @@
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="15" t="s">
-        <v>395</v>
+        <v>297</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
@@ -5445,27 +5454,27 @@
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
@@ -5499,32 +5508,32 @@
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="14" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="14" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="14" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="14" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="14" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="14" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
@@ -5537,17 +5546,17 @@
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="14" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="14" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="14" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
@@ -5562,17 +5571,17 @@
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="14" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="14" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="14" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
@@ -5590,22 +5599,22 @@
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="14" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="14" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="14" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="14" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
@@ -5638,12 +5647,12 @@
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="14" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
@@ -5661,17 +5670,17 @@
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="14" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="14" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="14" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
@@ -5679,7 +5688,7 @@
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="15" t="s">
-        <v>415</v>
+        <v>298</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
@@ -5689,7 +5698,7 @@
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" s="7" t="s">
-        <v>416</v>
+        <v>299</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
@@ -5699,7 +5708,7 @@
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="15" t="s">
-        <v>417</v>
+        <v>300</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
@@ -5725,27 +5734,27 @@
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
@@ -5784,32 +5793,32 @@
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" s="14" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="14" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="14" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" s="14" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="14" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="14" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
@@ -5822,17 +5831,17 @@
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="14" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" s="14" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="14" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
@@ -5847,17 +5856,17 @@
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="14" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="14" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" s="14" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
@@ -5875,27 +5884,27 @@
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="14" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="14" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" s="14" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="14" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="14" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
@@ -5928,12 +5937,12 @@
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" s="14" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
@@ -5951,17 +5960,17 @@
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" s="14" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" s="14" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" s="14" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
@@ -5969,7 +5978,7 @@
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" s="15" t="s">
-        <v>439</v>
+        <v>302</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
@@ -5979,7 +5988,7 @@
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" s="7" t="s">
-        <v>440</v>
+        <v>303</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
@@ -5989,7 +5998,7 @@
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" s="15" t="s">
-        <v>441</v>
+        <v>304</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
@@ -6015,27 +6024,27 @@
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" s="14" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" s="14" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" s="14" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
@@ -6074,37 +6083,37 @@
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" s="14" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" s="14" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" s="14" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" s="14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
@@ -6117,17 +6126,17 @@
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" s="14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" s="14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" s="14" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
@@ -6142,17 +6151,17 @@
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" s="14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" s="14" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" s="14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
@@ -6170,32 +6179,32 @@
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" s="14" t="s">
-        <v>256</v>
+        <v>453</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
@@ -6228,12 +6237,12 @@
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
@@ -6251,17 +6260,17 @@
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>